<commit_message>
complete rfe for peakachu k562; cross cell line  models for arrowhead gm12878 and k562
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_miscellaneous\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6A22CE-8558-41AF-99F8-FE98C2E52F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C69157-828C-47F5-91A0-CC6F26048D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="863" activeTab="2" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
+    <workbookView xWindow="12340" yWindow="3840" windowWidth="2820" windowHeight="1080" tabRatio="863" firstSheet="2" activeTab="3" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="TADRF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -564,7 +564,7 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView zoomScale="59" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855C5308-3D3F-4CB4-BE1D-ACF7EB36D075}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1449,6 +1449,9 @@
       </c>
       <c r="D13" t="s">
         <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1460,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67BA065-BC80-42CC-9885-44381DE0CC15}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1494,8 +1497,14 @@
       <c r="A4" t="s">
         <v>20</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
       <c r="D4" t="s">
         <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.75">
@@ -1556,7 +1565,7 @@
   <dimension ref="A1:Q115"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:C115"/>
+      <selection activeCell="B2" sqref="B2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
completed and initialized jobs for preciseTAD using arrowhead k562
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C69157-828C-47F5-91A0-CC6F26048D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE224FD5-D211-448E-AD39-93D908C0B979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="3840" windowWidth="2820" windowHeight="1080" tabRatio="863" firstSheet="2" activeTab="3" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
+    <workbookView xWindow="-28920" yWindow="9075" windowWidth="29040" windowHeight="15840" tabRatio="863" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="TADRF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -1463,7 +1463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67BA065-BC80-42CC-9885-44381DE0CC15}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1564,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1460CBE3-6AC6-450C-B58A-A9D559677404}">
   <dimension ref="A1:Q115"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B23"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1880,6 +1880,9 @@
       <c r="D13" t="s">
         <v>31</v>
       </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
       <c r="G13" t="s">
         <v>31</v>
       </c>
@@ -1906,6 +1909,9 @@
       <c r="D14" t="s">
         <v>32</v>
       </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
       <c r="G14" t="s">
         <v>32</v>
       </c>
@@ -1932,6 +1938,9 @@
       <c r="D15" t="s">
         <v>33</v>
       </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
       <c r="G15" t="s">
         <v>33</v>
       </c>
@@ -1958,6 +1967,9 @@
       <c r="D16" t="s">
         <v>34</v>
       </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
       <c r="G16" t="s">
         <v>34</v>
       </c>
@@ -1984,6 +1996,9 @@
       <c r="D17" t="s">
         <v>35</v>
       </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
       <c r="G17" t="s">
         <v>35</v>
       </c>
@@ -2010,6 +2025,9 @@
       <c r="D18" t="s">
         <v>36</v>
       </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
       <c r="G18" t="s">
         <v>36</v>
       </c>
@@ -2036,6 +2054,9 @@
       <c r="D19" t="s">
         <v>37</v>
       </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
       <c r="G19" t="s">
         <v>37</v>
       </c>
@@ -2062,6 +2083,9 @@
       <c r="D20" t="s">
         <v>38</v>
       </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
       <c r="G20" t="s">
         <v>38</v>
       </c>
@@ -2091,6 +2115,9 @@
       <c r="D21" t="s">
         <v>39</v>
       </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
       <c r="G21" t="s">
         <v>39</v>
       </c>
@@ -2120,6 +2147,9 @@
       <c r="D22" t="s">
         <v>40</v>
       </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
       <c r="G22" t="s">
         <v>40</v>
       </c>
@@ -2148,6 +2178,9 @@
       </c>
       <c r="D23" t="s">
         <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
       </c>
       <c r="G23" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
finished jobs; initialized preciseTAD k562 chr4,3,2
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE224FD5-D211-448E-AD39-93D908C0B979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEE146D-9B7F-424A-9541-58ACA7731A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9075" windowWidth="29040" windowHeight="15840" tabRatio="863" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -1565,7 +1565,7 @@
   <dimension ref="A1:Q115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1646,6 +1646,9 @@
       <c r="D4" t="s">
         <v>22</v>
       </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
       <c r="G4" t="s">
         <v>22</v>
       </c>
@@ -1672,6 +1675,9 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
@@ -1698,6 +1704,9 @@
       <c r="D6" t="s">
         <v>24</v>
       </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
       <c r="G6" t="s">
         <v>24</v>
       </c>
@@ -1724,6 +1733,9 @@
       <c r="D7" t="s">
         <v>25</v>
       </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
       <c r="G7" t="s">
         <v>25</v>
       </c>
@@ -1750,6 +1762,9 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
       <c r="G8" t="s">
         <v>26</v>
       </c>
@@ -1776,6 +1791,9 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
       <c r="G9" t="s">
         <v>27</v>
       </c>
@@ -1802,6 +1820,9 @@
       <c r="D10" t="s">
         <v>28</v>
       </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
       <c r="G10" t="s">
         <v>28</v>
       </c>
@@ -1828,6 +1849,9 @@
       <c r="D11" t="s">
         <v>29</v>
       </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
       <c r="G11" t="s">
         <v>29</v>
       </c>
@@ -1854,6 +1878,9 @@
       <c r="D12" t="s">
         <v>30</v>
       </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
       <c r="G12" t="s">
         <v>30</v>
       </c>
@@ -1881,7 +1908,7 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
         <v>31</v>
@@ -1939,7 +1966,7 @@
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s">
         <v>33</v>
@@ -3444,7 +3471,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
finished chr4,3, initialized chr1
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEE146D-9B7F-424A-9541-58ACA7731A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED7B15C-EE27-41FE-B591-C83F02E1E758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9075" windowWidth="29040" windowHeight="15840" tabRatio="863" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
+    <workbookView xWindow="-40455" yWindow="11580" windowWidth="21600" windowHeight="10890" tabRatio="863" firstSheet="2" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="TADRF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -1468,6 +1468,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="3" max="3" width="23.04296875" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -1564,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1460CBE3-6AC6-450C-B58A-A9D559677404}">
   <dimension ref="A1:Q115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1620,6 +1624,9 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
@@ -1676,7 +1683,7 @@
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -1705,7 +1712,7 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
completed precisetad chr22 on k562 arrowhead; initialized precisetad chr15-chr22 k562 peakachu
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED7B15C-EE27-41FE-B591-C83F02E1E758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CF06F4-F63E-4950-A1D6-0CA603B08DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40455" yWindow="11580" windowWidth="21600" windowHeight="10890" tabRatio="863" firstSheet="2" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="863" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="TADRF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -1464,7 +1464,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1569,7 +1569,7 @@
   <dimension ref="A1:Q115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1654,7 +1654,7 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -2019,8 +2019,11 @@
       <c r="P16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2048,8 +2051,11 @@
       <c r="P17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2077,8 +2083,11 @@
       <c r="P18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -2106,8 +2115,11 @@
       <c r="P19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2138,8 +2150,11 @@
       <c r="P20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2170,8 +2185,11 @@
       <c r="P21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2202,8 +2220,11 @@
       <c r="P22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -2234,8 +2255,11 @@
       <c r="P23" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.75">
+      <c r="Q23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -2249,7 +2273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -2263,7 +2287,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2277,7 +2301,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -2291,7 +2315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2305,7 +2329,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -2319,7 +2343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -2333,7 +2357,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
completed some jobs in preciseTAD k563 peakachu; initialized others
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CF06F4-F63E-4950-A1D6-0CA603B08DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8A8ECA-0AB7-40BF-808B-EF1AA43FC777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="863" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -1569,7 +1569,7 @@
   <dimension ref="A1:Q115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1729,6 +1729,9 @@
       <c r="P6" t="s">
         <v>24</v>
       </c>
+      <c r="Q6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
@@ -1758,6 +1761,9 @@
       <c r="P7" t="s">
         <v>25</v>
       </c>
+      <c r="Q7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
@@ -1787,6 +1793,9 @@
       <c r="P8" t="s">
         <v>26</v>
       </c>
+      <c r="Q8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
@@ -1816,6 +1825,9 @@
       <c r="P9" t="s">
         <v>27</v>
       </c>
+      <c r="Q9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
@@ -1845,6 +1857,9 @@
       <c r="P10" t="s">
         <v>28</v>
       </c>
+      <c r="Q10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
@@ -1874,6 +1889,9 @@
       <c r="P11" t="s">
         <v>29</v>
       </c>
+      <c r="Q11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
@@ -1903,6 +1921,9 @@
       <c r="P12" t="s">
         <v>30</v>
       </c>
+      <c r="Q12" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
@@ -1932,6 +1953,9 @@
       <c r="P13" t="s">
         <v>31</v>
       </c>
+      <c r="Q13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
@@ -1961,6 +1985,9 @@
       <c r="P14" t="s">
         <v>32</v>
       </c>
+      <c r="Q14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
@@ -1990,6 +2017,9 @@
       <c r="P15" t="s">
         <v>33</v>
       </c>
+      <c r="Q15" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
@@ -2020,7 +2050,7 @@
         <v>34</v>
       </c>
       <c r="Q16" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.75">
@@ -2052,7 +2082,7 @@
         <v>35</v>
       </c>
       <c r="Q17" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.75">
@@ -2084,7 +2114,7 @@
         <v>36</v>
       </c>
       <c r="Q18" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.75">
@@ -2116,7 +2146,7 @@
         <v>37</v>
       </c>
       <c r="Q19" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.75">
@@ -2151,7 +2181,7 @@
         <v>38</v>
       </c>
       <c r="Q20" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.75">
@@ -2186,7 +2216,7 @@
         <v>39</v>
       </c>
       <c r="Q21" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.75">
@@ -2221,7 +2251,7 @@
         <v>40</v>
       </c>
       <c r="Q22" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.75">
@@ -2256,7 +2286,7 @@
         <v>41</v>
       </c>
       <c r="Q23" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
initialized cross-cell line jobs for peakachu gm12878 chr1-chr22
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8A8ECA-0AB7-40BF-808B-EF1AA43FC777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAD484F-FA0C-4E8F-A6FC-9E09FD51D25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="863" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="863" activeTab="3" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="TADRF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67BA065-BC80-42CC-9885-44381DE0CC15}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1555,6 +1555,9 @@
       <c r="A14" t="s">
         <v>20</v>
       </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
@@ -1568,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1460CBE3-6AC6-450C-B58A-A9D559677404}">
   <dimension ref="A1:Q115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished some preciseTAD peakachu k562 jobs; initialized the rest for chr1-3; finished all cross cell line jobs for spectralTAD; initialized preciseTAD on spectralTAD gm12878 chr18-chr10
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAD484F-FA0C-4E8F-A6FC-9E09FD51D25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78344177-E975-4562-8487-A188400FADEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="863" activeTab="3" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="863" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="TADRF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67BA065-BC80-42CC-9885-44381DE0CC15}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1531,8 +1531,14 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
       <c r="D9" t="s">
         <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.75">
@@ -1556,10 +1562,13 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1571,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1460CBE3-6AC6-450C-B58A-A9D559677404}">
   <dimension ref="A1:Q115"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1645,6 +1654,9 @@
       <c r="P3" t="s">
         <v>21</v>
       </c>
+      <c r="Q3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
@@ -1674,6 +1686,9 @@
       <c r="P4" t="s">
         <v>22</v>
       </c>
+      <c r="Q4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
@@ -1703,6 +1718,9 @@
       <c r="P5" t="s">
         <v>23</v>
       </c>
+      <c r="Q5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
@@ -1733,7 +1751,7 @@
         <v>24</v>
       </c>
       <c r="Q6" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.75">
@@ -1765,7 +1783,7 @@
         <v>25</v>
       </c>
       <c r="Q7" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.75">
@@ -1797,7 +1815,7 @@
         <v>26</v>
       </c>
       <c r="Q8" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.75">
@@ -1829,7 +1847,7 @@
         <v>27</v>
       </c>
       <c r="Q9" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.75">
@@ -1880,6 +1898,9 @@
       <c r="G11" t="s">
         <v>29</v>
       </c>
+      <c r="H11" t="s">
+        <v>48</v>
+      </c>
       <c r="J11" t="s">
         <v>29</v>
       </c>
@@ -1912,6 +1933,9 @@
       <c r="G12" t="s">
         <v>30</v>
       </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
       <c r="J12" t="s">
         <v>30</v>
       </c>
@@ -1925,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="Q12" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.75">
@@ -1944,6 +1968,9 @@
       <c r="G13" t="s">
         <v>31</v>
       </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
       <c r="J13" t="s">
         <v>31</v>
       </c>
@@ -1976,6 +2003,9 @@
       <c r="G14" t="s">
         <v>32</v>
       </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
       <c r="J14" t="s">
         <v>32</v>
       </c>
@@ -2008,6 +2038,9 @@
       <c r="G15" t="s">
         <v>33</v>
       </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
       <c r="J15" t="s">
         <v>33</v>
       </c>
@@ -2040,6 +2073,9 @@
       <c r="G16" t="s">
         <v>34</v>
       </c>
+      <c r="H16" t="s">
+        <v>48</v>
+      </c>
       <c r="J16" t="s">
         <v>34</v>
       </c>
@@ -2072,6 +2108,9 @@
       <c r="G17" t="s">
         <v>35</v>
       </c>
+      <c r="H17" t="s">
+        <v>48</v>
+      </c>
       <c r="J17" t="s">
         <v>35</v>
       </c>
@@ -2104,6 +2143,9 @@
       <c r="G18" t="s">
         <v>36</v>
       </c>
+      <c r="H18" t="s">
+        <v>48</v>
+      </c>
       <c r="J18" t="s">
         <v>36</v>
       </c>
@@ -2135,6 +2177,9 @@
       </c>
       <c r="G19" t="s">
         <v>37</v>
+      </c>
+      <c r="H19" t="s">
+        <v>48</v>
       </c>
       <c r="J19" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
completed jobs; initialized the rest of preciseTAD jobs for gm12878 and k562 using arrowhead for other resolutions (10kb-100kb); all total 2*4*21 jobs
</commit_message>
<xml_diff>
--- a/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
+++ b/jobs_left_to_run/number_of_scripts_to_run_nminus1_chr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\Documents\TAD_predictive_modeling\jobs_left_to_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78344177-E975-4562-8487-A188400FADEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC96659-A3C0-4043-B52D-408574C7A031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="863" activeTab="4" xr2:uid="{F551FBCC-C783-459F-A691-DCC8687BDF6E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -1581,7 +1581,7 @@
   <dimension ref="A1:Q115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E95" sqref="E95:E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1637,10 +1637,13 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
       </c>
       <c r="J3" t="s">
         <v>21</v>
@@ -1674,6 +1677,9 @@
       <c r="G4" t="s">
         <v>22</v>
       </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
@@ -1706,6 +1712,9 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
       <c r="J5" t="s">
         <v>23</v>
       </c>
@@ -1719,7 +1728,7 @@
         <v>23</v>
       </c>
       <c r="Q5" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.75">
@@ -1738,6 +1747,9 @@
       <c r="G6" t="s">
         <v>24</v>
       </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
       <c r="J6" t="s">
         <v>24</v>
       </c>
@@ -1770,6 +1782,9 @@
       <c r="G7" t="s">
         <v>25</v>
       </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
       <c r="J7" t="s">
         <v>25</v>
       </c>
@@ -1802,6 +1817,9 @@
       <c r="G8" t="s">
         <v>26</v>
       </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
       <c r="J8" t="s">
         <v>26</v>
       </c>
@@ -1834,6 +1852,9 @@
       <c r="G9" t="s">
         <v>27</v>
       </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
       <c r="J9" t="s">
         <v>27</v>
       </c>
@@ -1866,6 +1887,9 @@
       <c r="G10" t="s">
         <v>28</v>
       </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
       <c r="J10" t="s">
         <v>28</v>
       </c>
@@ -1899,7 +1923,7 @@
         <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J11" t="s">
         <v>29</v>
@@ -1934,7 +1958,7 @@
         <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
         <v>30</v>
@@ -1969,7 +1993,7 @@
         <v>31</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J13" t="s">
         <v>31</v>
@@ -2004,7 +2028,7 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J14" t="s">
         <v>32</v>
@@ -2039,7 +2063,7 @@
         <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J15" t="s">
         <v>33</v>
@@ -2074,7 +2098,7 @@
         <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J16" t="s">
         <v>34</v>
@@ -2109,7 +2133,7 @@
         <v>35</v>
       </c>
       <c r="H17" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J17" t="s">
         <v>35</v>
@@ -2144,7 +2168,7 @@
         <v>36</v>
       </c>
       <c r="H18" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J18" t="s">
         <v>36</v>
@@ -2179,7 +2203,7 @@
         <v>37</v>
       </c>
       <c r="H19" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J19" t="s">
         <v>37</v>
@@ -2355,8 +2379,14 @@
       <c r="A26" t="s">
         <v>21</v>
       </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
       <c r="D26" t="s">
         <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
       </c>
       <c r="G26" t="s">
         <v>21</v>
@@ -2369,8 +2399,14 @@
       <c r="A27" t="s">
         <v>22</v>
       </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
       <c r="D27" t="s">
         <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
@@ -2383,8 +2419,14 @@
       <c r="A28" t="s">
         <v>23</v>
       </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
       <c r="D28" t="s">
         <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
       </c>
       <c r="G28" t="s">
         <v>23</v>
@@ -2397,8 +2439,14 @@
       <c r="A29" t="s">
         <v>24</v>
       </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
       <c r="D29" t="s">
         <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
       </c>
       <c r="G29" t="s">
         <v>24</v>
@@ -2411,8 +2459,14 @@
       <c r="A30" t="s">
         <v>25</v>
       </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
       <c r="D30" t="s">
         <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>48</v>
       </c>
       <c r="G30" t="s">
         <v>25</v>
@@ -2425,8 +2479,14 @@
       <c r="A31" t="s">
         <v>26</v>
       </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
       <c r="D31" t="s">
         <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>48</v>
       </c>
       <c r="G31" t="s">
         <v>26</v>
@@ -2439,8 +2499,14 @@
       <c r="A32" t="s">
         <v>27</v>
       </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
       <c r="D32" t="s">
         <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
       </c>
       <c r="G32" t="s">
         <v>27</v>
@@ -2453,8 +2519,14 @@
       <c r="A33" t="s">
         <v>28</v>
       </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
       <c r="D33" t="s">
         <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
       </c>
       <c r="G33" t="s">
         <v>28</v>
@@ -2467,8 +2539,14 @@
       <c r="A34" t="s">
         <v>29</v>
       </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
       <c r="D34" t="s">
         <v>29</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
       </c>
       <c r="G34" t="s">
         <v>29</v>
@@ -2481,8 +2559,14 @@
       <c r="A35" t="s">
         <v>30</v>
       </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
       <c r="D35" t="s">
         <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
       </c>
       <c r="G35" t="s">
         <v>30</v>
@@ -2495,8 +2579,14 @@
       <c r="A36" t="s">
         <v>31</v>
       </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
       <c r="D36" t="s">
         <v>31</v>
+      </c>
+      <c r="E36" t="s">
+        <v>48</v>
       </c>
       <c r="G36" t="s">
         <v>31</v>
@@ -2509,8 +2599,14 @@
       <c r="A37" t="s">
         <v>32</v>
       </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
       <c r="D37" t="s">
         <v>32</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
       </c>
       <c r="G37" t="s">
         <v>32</v>
@@ -2523,8 +2619,14 @@
       <c r="A38" t="s">
         <v>33</v>
       </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
       <c r="D38" t="s">
         <v>33</v>
+      </c>
+      <c r="E38" t="s">
+        <v>48</v>
       </c>
       <c r="G38" t="s">
         <v>33</v>
@@ -2537,8 +2639,14 @@
       <c r="A39" t="s">
         <v>34</v>
       </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
       <c r="D39" t="s">
         <v>34</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
       </c>
       <c r="G39" t="s">
         <v>34</v>
@@ -2551,8 +2659,14 @@
       <c r="A40" t="s">
         <v>35</v>
       </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
       <c r="D40" t="s">
         <v>35</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
       </c>
       <c r="G40" t="s">
         <v>35</v>
@@ -2565,8 +2679,14 @@
       <c r="A41" t="s">
         <v>36</v>
       </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
       <c r="D41" t="s">
         <v>36</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
       </c>
       <c r="G41" t="s">
         <v>36</v>
@@ -2579,8 +2699,14 @@
       <c r="A42" t="s">
         <v>37</v>
       </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
       <c r="D42" t="s">
         <v>37</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
       </c>
       <c r="G42" t="s">
         <v>37</v>
@@ -2593,8 +2719,14 @@
       <c r="A43" t="s">
         <v>38</v>
       </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
       <c r="D43" t="s">
         <v>38</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
       </c>
       <c r="G43" t="s">
         <v>38</v>
@@ -2607,8 +2739,14 @@
       <c r="A44" t="s">
         <v>39</v>
       </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
       <c r="D44" t="s">
         <v>39</v>
+      </c>
+      <c r="E44" t="s">
+        <v>48</v>
       </c>
       <c r="G44" t="s">
         <v>39</v>
@@ -2621,8 +2759,14 @@
       <c r="A45" t="s">
         <v>40</v>
       </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
       <c r="D45" t="s">
         <v>40</v>
+      </c>
+      <c r="E45" t="s">
+        <v>48</v>
       </c>
       <c r="G45" t="s">
         <v>40</v>
@@ -2635,8 +2779,14 @@
       <c r="A46" t="s">
         <v>41</v>
       </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
       <c r="D46" t="s">
         <v>41</v>
+      </c>
+      <c r="E46" t="s">
+        <v>48</v>
       </c>
       <c r="G46" t="s">
         <v>41</v>
@@ -2663,8 +2813,14 @@
       <c r="A49" t="s">
         <v>21</v>
       </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
       <c r="D49" t="s">
         <v>21</v>
+      </c>
+      <c r="E49" t="s">
+        <v>48</v>
       </c>
       <c r="G49" t="s">
         <v>21</v>
@@ -2677,8 +2833,14 @@
       <c r="A50" t="s">
         <v>22</v>
       </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
       <c r="D50" t="s">
         <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>48</v>
       </c>
       <c r="G50" t="s">
         <v>22</v>
@@ -2691,8 +2853,14 @@
       <c r="A51" t="s">
         <v>23</v>
       </c>
+      <c r="B51" t="s">
+        <v>48</v>
+      </c>
       <c r="D51" t="s">
         <v>23</v>
+      </c>
+      <c r="E51" t="s">
+        <v>48</v>
       </c>
       <c r="G51" t="s">
         <v>23</v>
@@ -2705,8 +2873,14 @@
       <c r="A52" t="s">
         <v>24</v>
       </c>
+      <c r="B52" t="s">
+        <v>48</v>
+      </c>
       <c r="D52" t="s">
         <v>24</v>
+      </c>
+      <c r="E52" t="s">
+        <v>48</v>
       </c>
       <c r="G52" t="s">
         <v>24</v>
@@ -2719,8 +2893,14 @@
       <c r="A53" t="s">
         <v>25</v>
       </c>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
       <c r="D53" t="s">
         <v>25</v>
+      </c>
+      <c r="E53" t="s">
+        <v>48</v>
       </c>
       <c r="G53" t="s">
         <v>25</v>
@@ -2733,8 +2913,14 @@
       <c r="A54" t="s">
         <v>26</v>
       </c>
+      <c r="B54" t="s">
+        <v>48</v>
+      </c>
       <c r="D54" t="s">
         <v>26</v>
+      </c>
+      <c r="E54" t="s">
+        <v>48</v>
       </c>
       <c r="G54" t="s">
         <v>26</v>
@@ -2747,8 +2933,14 @@
       <c r="A55" t="s">
         <v>27</v>
       </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
       <c r="D55" t="s">
         <v>27</v>
+      </c>
+      <c r="E55" t="s">
+        <v>48</v>
       </c>
       <c r="G55" t="s">
         <v>27</v>
@@ -2761,8 +2953,14 @@
       <c r="A56" t="s">
         <v>28</v>
       </c>
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
       <c r="D56" t="s">
         <v>28</v>
+      </c>
+      <c r="E56" t="s">
+        <v>48</v>
       </c>
       <c r="G56" t="s">
         <v>28</v>
@@ -2775,8 +2973,14 @@
       <c r="A57" t="s">
         <v>29</v>
       </c>
+      <c r="B57" t="s">
+        <v>48</v>
+      </c>
       <c r="D57" t="s">
         <v>29</v>
+      </c>
+      <c r="E57" t="s">
+        <v>48</v>
       </c>
       <c r="G57" t="s">
         <v>29</v>
@@ -2789,8 +2993,14 @@
       <c r="A58" t="s">
         <v>30</v>
       </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
       <c r="D58" t="s">
         <v>30</v>
+      </c>
+      <c r="E58" t="s">
+        <v>48</v>
       </c>
       <c r="G58" t="s">
         <v>30</v>
@@ -2803,8 +3013,14 @@
       <c r="A59" t="s">
         <v>31</v>
       </c>
+      <c r="B59" t="s">
+        <v>48</v>
+      </c>
       <c r="D59" t="s">
         <v>31</v>
+      </c>
+      <c r="E59" t="s">
+        <v>48</v>
       </c>
       <c r="G59" t="s">
         <v>31</v>
@@ -2817,8 +3033,14 @@
       <c r="A60" t="s">
         <v>32</v>
       </c>
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
       <c r="D60" t="s">
         <v>32</v>
+      </c>
+      <c r="E60" t="s">
+        <v>48</v>
       </c>
       <c r="G60" t="s">
         <v>32</v>
@@ -2831,8 +3053,14 @@
       <c r="A61" t="s">
         <v>33</v>
       </c>
+      <c r="B61" t="s">
+        <v>48</v>
+      </c>
       <c r="D61" t="s">
         <v>33</v>
+      </c>
+      <c r="E61" t="s">
+        <v>48</v>
       </c>
       <c r="G61" t="s">
         <v>33</v>
@@ -2845,8 +3073,14 @@
       <c r="A62" t="s">
         <v>34</v>
       </c>
+      <c r="B62" t="s">
+        <v>48</v>
+      </c>
       <c r="D62" t="s">
         <v>34</v>
+      </c>
+      <c r="E62" t="s">
+        <v>48</v>
       </c>
       <c r="G62" t="s">
         <v>34</v>
@@ -2859,8 +3093,14 @@
       <c r="A63" t="s">
         <v>35</v>
       </c>
+      <c r="B63" t="s">
+        <v>48</v>
+      </c>
       <c r="D63" t="s">
         <v>35</v>
+      </c>
+      <c r="E63" t="s">
+        <v>48</v>
       </c>
       <c r="G63" t="s">
         <v>35</v>
@@ -2873,8 +3113,14 @@
       <c r="A64" t="s">
         <v>36</v>
       </c>
+      <c r="B64" t="s">
+        <v>48</v>
+      </c>
       <c r="D64" t="s">
         <v>36</v>
+      </c>
+      <c r="E64" t="s">
+        <v>48</v>
       </c>
       <c r="G64" t="s">
         <v>36</v>
@@ -2887,8 +3133,14 @@
       <c r="A65" t="s">
         <v>37</v>
       </c>
+      <c r="B65" t="s">
+        <v>48</v>
+      </c>
       <c r="D65" t="s">
         <v>37</v>
+      </c>
+      <c r="E65" t="s">
+        <v>48</v>
       </c>
       <c r="G65" t="s">
         <v>37</v>
@@ -2901,8 +3153,14 @@
       <c r="A66" t="s">
         <v>38</v>
       </c>
+      <c r="B66" t="s">
+        <v>48</v>
+      </c>
       <c r="D66" t="s">
         <v>38</v>
+      </c>
+      <c r="E66" t="s">
+        <v>48</v>
       </c>
       <c r="G66" t="s">
         <v>38</v>
@@ -2915,8 +3173,14 @@
       <c r="A67" t="s">
         <v>39</v>
       </c>
+      <c r="B67" t="s">
+        <v>48</v>
+      </c>
       <c r="D67" t="s">
         <v>39</v>
+      </c>
+      <c r="E67" t="s">
+        <v>48</v>
       </c>
       <c r="G67" t="s">
         <v>39</v>
@@ -2929,8 +3193,14 @@
       <c r="A68" t="s">
         <v>40</v>
       </c>
+      <c r="B68" t="s">
+        <v>48</v>
+      </c>
       <c r="D68" t="s">
         <v>40</v>
+      </c>
+      <c r="E68" t="s">
+        <v>48</v>
       </c>
       <c r="G68" t="s">
         <v>40</v>
@@ -2943,8 +3213,14 @@
       <c r="A69" t="s">
         <v>41</v>
       </c>
+      <c r="B69" t="s">
+        <v>48</v>
+      </c>
       <c r="D69" t="s">
         <v>41</v>
+      </c>
+      <c r="E69" t="s">
+        <v>48</v>
       </c>
       <c r="G69" t="s">
         <v>41</v>
@@ -2971,8 +3247,14 @@
       <c r="A72" t="s">
         <v>21</v>
       </c>
+      <c r="B72" t="s">
+        <v>48</v>
+      </c>
       <c r="D72" t="s">
         <v>21</v>
+      </c>
+      <c r="E72" t="s">
+        <v>48</v>
       </c>
       <c r="G72" t="s">
         <v>21</v>
@@ -2985,8 +3267,14 @@
       <c r="A73" t="s">
         <v>22</v>
       </c>
+      <c r="B73" t="s">
+        <v>48</v>
+      </c>
       <c r="D73" t="s">
         <v>22</v>
+      </c>
+      <c r="E73" t="s">
+        <v>48</v>
       </c>
       <c r="G73" t="s">
         <v>22</v>
@@ -2999,8 +3287,14 @@
       <c r="A74" t="s">
         <v>23</v>
       </c>
+      <c r="B74" t="s">
+        <v>48</v>
+      </c>
       <c r="D74" t="s">
         <v>23</v>
+      </c>
+      <c r="E74" t="s">
+        <v>48</v>
       </c>
       <c r="G74" t="s">
         <v>23</v>
@@ -3013,8 +3307,14 @@
       <c r="A75" t="s">
         <v>24</v>
       </c>
+      <c r="B75" t="s">
+        <v>48</v>
+      </c>
       <c r="D75" t="s">
         <v>24</v>
+      </c>
+      <c r="E75" t="s">
+        <v>48</v>
       </c>
       <c r="G75" t="s">
         <v>24</v>
@@ -3027,8 +3327,14 @@
       <c r="A76" t="s">
         <v>25</v>
       </c>
+      <c r="B76" t="s">
+        <v>48</v>
+      </c>
       <c r="D76" t="s">
         <v>25</v>
+      </c>
+      <c r="E76" t="s">
+        <v>48</v>
       </c>
       <c r="G76" t="s">
         <v>25</v>
@@ -3041,8 +3347,14 @@
       <c r="A77" t="s">
         <v>26</v>
       </c>
+      <c r="B77" t="s">
+        <v>48</v>
+      </c>
       <c r="D77" t="s">
         <v>26</v>
+      </c>
+      <c r="E77" t="s">
+        <v>48</v>
       </c>
       <c r="G77" t="s">
         <v>26</v>
@@ -3055,8 +3367,14 @@
       <c r="A78" t="s">
         <v>27</v>
       </c>
+      <c r="B78" t="s">
+        <v>48</v>
+      </c>
       <c r="D78" t="s">
         <v>27</v>
+      </c>
+      <c r="E78" t="s">
+        <v>48</v>
       </c>
       <c r="G78" t="s">
         <v>27</v>
@@ -3069,8 +3387,14 @@
       <c r="A79" t="s">
         <v>28</v>
       </c>
+      <c r="B79" t="s">
+        <v>48</v>
+      </c>
       <c r="D79" t="s">
         <v>28</v>
+      </c>
+      <c r="E79" t="s">
+        <v>48</v>
       </c>
       <c r="G79" t="s">
         <v>28</v>
@@ -3083,8 +3407,14 @@
       <c r="A80" t="s">
         <v>29</v>
       </c>
+      <c r="B80" t="s">
+        <v>48</v>
+      </c>
       <c r="D80" t="s">
         <v>29</v>
+      </c>
+      <c r="E80" t="s">
+        <v>48</v>
       </c>
       <c r="G80" t="s">
         <v>29</v>
@@ -3097,8 +3427,14 @@
       <c r="A81" t="s">
         <v>30</v>
       </c>
+      <c r="B81" t="s">
+        <v>48</v>
+      </c>
       <c r="D81" t="s">
         <v>30</v>
+      </c>
+      <c r="E81" t="s">
+        <v>48</v>
       </c>
       <c r="G81" t="s">
         <v>30</v>
@@ -3111,8 +3447,14 @@
       <c r="A82" t="s">
         <v>31</v>
       </c>
+      <c r="B82" t="s">
+        <v>48</v>
+      </c>
       <c r="D82" t="s">
         <v>31</v>
+      </c>
+      <c r="E82" t="s">
+        <v>48</v>
       </c>
       <c r="G82" t="s">
         <v>31</v>
@@ -3125,8 +3467,14 @@
       <c r="A83" t="s">
         <v>32</v>
       </c>
+      <c r="B83" t="s">
+        <v>48</v>
+      </c>
       <c r="D83" t="s">
         <v>32</v>
+      </c>
+      <c r="E83" t="s">
+        <v>48</v>
       </c>
       <c r="G83" t="s">
         <v>32</v>
@@ -3139,8 +3487,14 @@
       <c r="A84" t="s">
         <v>33</v>
       </c>
+      <c r="B84" t="s">
+        <v>48</v>
+      </c>
       <c r="D84" t="s">
         <v>33</v>
+      </c>
+      <c r="E84" t="s">
+        <v>48</v>
       </c>
       <c r="G84" t="s">
         <v>33</v>
@@ -3153,8 +3507,14 @@
       <c r="A85" t="s">
         <v>34</v>
       </c>
+      <c r="B85" t="s">
+        <v>48</v>
+      </c>
       <c r="D85" t="s">
         <v>34</v>
+      </c>
+      <c r="E85" t="s">
+        <v>48</v>
       </c>
       <c r="G85" t="s">
         <v>34</v>
@@ -3167,8 +3527,14 @@
       <c r="A86" t="s">
         <v>35</v>
       </c>
+      <c r="B86" t="s">
+        <v>48</v>
+      </c>
       <c r="D86" t="s">
         <v>35</v>
+      </c>
+      <c r="E86" t="s">
+        <v>48</v>
       </c>
       <c r="G86" t="s">
         <v>35</v>
@@ -3181,8 +3547,14 @@
       <c r="A87" t="s">
         <v>36</v>
       </c>
+      <c r="B87" t="s">
+        <v>48</v>
+      </c>
       <c r="D87" t="s">
         <v>36</v>
+      </c>
+      <c r="E87" t="s">
+        <v>48</v>
       </c>
       <c r="G87" t="s">
         <v>36</v>
@@ -3195,8 +3567,14 @@
       <c r="A88" t="s">
         <v>37</v>
       </c>
+      <c r="B88" t="s">
+        <v>48</v>
+      </c>
       <c r="D88" t="s">
         <v>37</v>
+      </c>
+      <c r="E88" t="s">
+        <v>48</v>
       </c>
       <c r="G88" t="s">
         <v>37</v>
@@ -3209,8 +3587,14 @@
       <c r="A89" t="s">
         <v>38</v>
       </c>
+      <c r="B89" t="s">
+        <v>48</v>
+      </c>
       <c r="D89" t="s">
         <v>38</v>
+      </c>
+      <c r="E89" t="s">
+        <v>48</v>
       </c>
       <c r="G89" t="s">
         <v>38</v>
@@ -3223,8 +3607,14 @@
       <c r="A90" t="s">
         <v>39</v>
       </c>
+      <c r="B90" t="s">
+        <v>48</v>
+      </c>
       <c r="D90" t="s">
         <v>39</v>
+      </c>
+      <c r="E90" t="s">
+        <v>48</v>
       </c>
       <c r="G90" t="s">
         <v>39</v>
@@ -3237,8 +3627,14 @@
       <c r="A91" t="s">
         <v>40</v>
       </c>
+      <c r="B91" t="s">
+        <v>48</v>
+      </c>
       <c r="D91" t="s">
         <v>40</v>
+      </c>
+      <c r="E91" t="s">
+        <v>48</v>
       </c>
       <c r="G91" t="s">
         <v>40</v>
@@ -3251,8 +3647,14 @@
       <c r="A92" t="s">
         <v>41</v>
       </c>
+      <c r="B92" t="s">
+        <v>48</v>
+      </c>
       <c r="D92" t="s">
         <v>41</v>
+      </c>
+      <c r="E92" t="s">
+        <v>48</v>
       </c>
       <c r="G92" t="s">
         <v>41</v>
@@ -3279,8 +3681,14 @@
       <c r="A95" t="s">
         <v>21</v>
       </c>
+      <c r="B95" t="s">
+        <v>48</v>
+      </c>
       <c r="D95" t="s">
         <v>21</v>
+      </c>
+      <c r="E95" t="s">
+        <v>48</v>
       </c>
       <c r="G95" t="s">
         <v>21</v>
@@ -3293,8 +3701,14 @@
       <c r="A96" t="s">
         <v>22</v>
       </c>
+      <c r="B96" t="s">
+        <v>48</v>
+      </c>
       <c r="D96" t="s">
         <v>22</v>
+      </c>
+      <c r="E96" t="s">
+        <v>48</v>
       </c>
       <c r="G96" t="s">
         <v>22</v>
@@ -3307,8 +3721,14 @@
       <c r="A97" t="s">
         <v>23</v>
       </c>
+      <c r="B97" t="s">
+        <v>48</v>
+      </c>
       <c r="D97" t="s">
         <v>23</v>
+      </c>
+      <c r="E97" t="s">
+        <v>48</v>
       </c>
       <c r="G97" t="s">
         <v>23</v>
@@ -3321,8 +3741,14 @@
       <c r="A98" t="s">
         <v>24</v>
       </c>
+      <c r="B98" t="s">
+        <v>48</v>
+      </c>
       <c r="D98" t="s">
         <v>24</v>
+      </c>
+      <c r="E98" t="s">
+        <v>48</v>
       </c>
       <c r="G98" t="s">
         <v>24</v>
@@ -3335,8 +3761,14 @@
       <c r="A99" t="s">
         <v>25</v>
       </c>
+      <c r="B99" t="s">
+        <v>48</v>
+      </c>
       <c r="D99" t="s">
         <v>25</v>
+      </c>
+      <c r="E99" t="s">
+        <v>48</v>
       </c>
       <c r="G99" t="s">
         <v>25</v>
@@ -3349,8 +3781,14 @@
       <c r="A100" t="s">
         <v>26</v>
       </c>
+      <c r="B100" t="s">
+        <v>48</v>
+      </c>
       <c r="D100" t="s">
         <v>26</v>
+      </c>
+      <c r="E100" t="s">
+        <v>48</v>
       </c>
       <c r="G100" t="s">
         <v>26</v>
@@ -3363,8 +3801,14 @@
       <c r="A101" t="s">
         <v>27</v>
       </c>
+      <c r="B101" t="s">
+        <v>48</v>
+      </c>
       <c r="D101" t="s">
         <v>27</v>
+      </c>
+      <c r="E101" t="s">
+        <v>48</v>
       </c>
       <c r="G101" t="s">
         <v>27</v>
@@ -3377,8 +3821,14 @@
       <c r="A102" t="s">
         <v>28</v>
       </c>
+      <c r="B102" t="s">
+        <v>48</v>
+      </c>
       <c r="D102" t="s">
         <v>28</v>
+      </c>
+      <c r="E102" t="s">
+        <v>48</v>
       </c>
       <c r="G102" t="s">
         <v>28</v>
@@ -3391,8 +3841,14 @@
       <c r="A103" t="s">
         <v>29</v>
       </c>
+      <c r="B103" t="s">
+        <v>48</v>
+      </c>
       <c r="D103" t="s">
         <v>29</v>
+      </c>
+      <c r="E103" t="s">
+        <v>48</v>
       </c>
       <c r="G103" t="s">
         <v>29</v>
@@ -3405,8 +3861,14 @@
       <c r="A104" t="s">
         <v>30</v>
       </c>
+      <c r="B104" t="s">
+        <v>48</v>
+      </c>
       <c r="D104" t="s">
         <v>30</v>
+      </c>
+      <c r="E104" t="s">
+        <v>48</v>
       </c>
       <c r="G104" t="s">
         <v>30</v>
@@ -3419,8 +3881,14 @@
       <c r="A105" t="s">
         <v>31</v>
       </c>
+      <c r="B105" t="s">
+        <v>48</v>
+      </c>
       <c r="D105" t="s">
         <v>31</v>
+      </c>
+      <c r="E105" t="s">
+        <v>48</v>
       </c>
       <c r="G105" t="s">
         <v>31</v>
@@ -3433,8 +3901,14 @@
       <c r="A106" t="s">
         <v>32</v>
       </c>
+      <c r="B106" t="s">
+        <v>48</v>
+      </c>
       <c r="D106" t="s">
         <v>32</v>
+      </c>
+      <c r="E106" t="s">
+        <v>48</v>
       </c>
       <c r="G106" t="s">
         <v>32</v>
@@ -3447,8 +3921,14 @@
       <c r="A107" t="s">
         <v>33</v>
       </c>
+      <c r="B107" t="s">
+        <v>48</v>
+      </c>
       <c r="D107" t="s">
         <v>33</v>
+      </c>
+      <c r="E107" t="s">
+        <v>48</v>
       </c>
       <c r="G107" t="s">
         <v>33</v>
@@ -3461,8 +3941,14 @@
       <c r="A108" t="s">
         <v>34</v>
       </c>
+      <c r="B108" t="s">
+        <v>48</v>
+      </c>
       <c r="D108" t="s">
         <v>34</v>
+      </c>
+      <c r="E108" t="s">
+        <v>48</v>
       </c>
       <c r="G108" t="s">
         <v>34</v>
@@ -3475,8 +3961,14 @@
       <c r="A109" t="s">
         <v>35</v>
       </c>
+      <c r="B109" t="s">
+        <v>48</v>
+      </c>
       <c r="D109" t="s">
         <v>35</v>
+      </c>
+      <c r="E109" t="s">
+        <v>48</v>
       </c>
       <c r="G109" t="s">
         <v>35</v>
@@ -3489,8 +3981,14 @@
       <c r="A110" t="s">
         <v>36</v>
       </c>
+      <c r="B110" t="s">
+        <v>48</v>
+      </c>
       <c r="D110" t="s">
         <v>36</v>
+      </c>
+      <c r="E110" t="s">
+        <v>48</v>
       </c>
       <c r="G110" t="s">
         <v>36</v>
@@ -3503,8 +4001,14 @@
       <c r="A111" t="s">
         <v>37</v>
       </c>
+      <c r="B111" t="s">
+        <v>48</v>
+      </c>
       <c r="D111" t="s">
         <v>37</v>
+      </c>
+      <c r="E111" t="s">
+        <v>48</v>
       </c>
       <c r="G111" t="s">
         <v>37</v>
@@ -3517,8 +4021,14 @@
       <c r="A112" t="s">
         <v>38</v>
       </c>
+      <c r="B112" t="s">
+        <v>48</v>
+      </c>
       <c r="D112" t="s">
         <v>38</v>
+      </c>
+      <c r="E112" t="s">
+        <v>48</v>
       </c>
       <c r="G112" t="s">
         <v>38</v>
@@ -3531,8 +4041,14 @@
       <c r="A113" t="s">
         <v>39</v>
       </c>
+      <c r="B113" t="s">
+        <v>48</v>
+      </c>
       <c r="D113" t="s">
         <v>39</v>
+      </c>
+      <c r="E113" t="s">
+        <v>48</v>
       </c>
       <c r="G113" t="s">
         <v>39</v>
@@ -3545,8 +4061,14 @@
       <c r="A114" t="s">
         <v>40</v>
       </c>
+      <c r="B114" t="s">
+        <v>48</v>
+      </c>
       <c r="D114" t="s">
         <v>40</v>
+      </c>
+      <c r="E114" t="s">
+        <v>48</v>
       </c>
       <c r="G114" t="s">
         <v>40</v>
@@ -3559,8 +4081,14 @@
       <c r="A115" t="s">
         <v>41</v>
       </c>
+      <c r="B115" t="s">
+        <v>48</v>
+      </c>
       <c r="D115" t="s">
         <v>41</v>
+      </c>
+      <c r="E115" t="s">
+        <v>48</v>
       </c>
       <c r="G115" t="s">
         <v>41</v>

</xml_diff>